<commit_message>
Updated budget sheet for car rentals
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Documents/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant\Desktop\Class Notes\Spring 2018\CS4320\CS4320TravelPlans\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,11 +14,8 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150000" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
   <si>
     <t>Travel</t>
   </si>
@@ -60,12 +57,18 @@
   </si>
   <si>
     <t>Expense</t>
+  </si>
+  <si>
+    <t>Car Rental (5 Exotic Cars)</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
+  </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -124,16 +127,17 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -143,6 +147,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -414,10 +421,10 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
     <col min="2" max="3" width="22.6640625" customWidth="1"/>
@@ -426,21 +433,21 @@
     <col min="7" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.35">
-      <c r="A1" s="1" t="s">
+    <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.7">
+      <c r="A1" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1" t="s">
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="1"/>
+      <c r="H1" s="3"/>
     </row>
-    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A2" s="4" t="s">
         <v>0</v>
       </c>
@@ -453,57 +460,63 @@
         <v>2</v>
       </c>
       <c r="F2" s="4"/>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="H2" s="3">
+      <c r="H2" s="2">
         <f>SUM(B4:B1048576)</f>
-        <v>0</v>
+        <v>59127</v>
       </c>
     </row>
-    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
+      <c r="D3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="E3" s="3" t="s">
+      <c r="E3" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="F3" s="3" t="s">
+      <c r="F3" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="2" t="s">
+      <c r="G3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H3" s="3">
+      <c r="H3" s="2">
         <f>SUM(D4:D1048576)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="G4" s="2" t="s">
+    <row r="4" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A4" t="s">
+        <v>11</v>
+      </c>
+      <c r="B4" s="5">
+        <v>59127</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="H4" s="3">
+      <c r="H4" s="2">
         <f>SUM(F4:F1048576)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
-      <c r="G5" s="2" t="s">
+    <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="H5" s="3">
+      <c r="H5" s="2">
         <f>SUM($H2, $H3, $H4)</f>
-        <v>0</v>
+        <v>59127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added plane ticket price to budget
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -1,21 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant\Desktop\Class Notes\Spring 2018\CS4320\CS4320TravelPlans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Documents/Software Engineering/CS4320TravelPlans/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14380" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="13">
   <si>
     <t>Travel</t>
   </si>
@@ -60,13 +63,17 @@
   </si>
   <si>
     <t>Car Rental (5 Exotic Cars)</t>
+  </si>
+  <si>
+    <t>Private Jet Rental</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="3" x14ac:knownFonts="1">
@@ -127,17 +134,18 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -421,10 +429,10 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
     <col min="2" max="3" width="22.6640625" customWidth="1"/>
@@ -434,38 +442,38 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.7">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
+      <c r="F1" s="4"/>
+      <c r="G1" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="H1" s="3"/>
+      <c r="H1" s="4"/>
     </row>
     <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
-      <c r="A2" s="4" t="s">
+      <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="4" t="s">
+      <c r="B2" s="5"/>
+      <c r="C2" s="5" t="s">
         <v>1</v>
       </c>
-      <c r="D2" s="4"/>
-      <c r="E2" s="4" t="s">
+      <c r="D2" s="5"/>
+      <c r="E2" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="F2" s="4"/>
+      <c r="F2" s="5"/>
       <c r="G2" s="1" t="s">
         <v>4</v>
       </c>
       <c r="H2" s="2">
         <f>SUM(B4:B1048576)</f>
-        <v>59127</v>
+        <v>77127</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
@@ -499,7 +507,7 @@
       <c r="A4" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="5">
+      <c r="B4" s="3">
         <v>59127</v>
       </c>
       <c r="G4" s="1" t="s">
@@ -511,12 +519,18 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+      <c r="A5" t="s">
+        <v>12</v>
+      </c>
+      <c r="B5" s="6">
+        <v>18000</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="2">
         <f>SUM($H2, $H3, $H4)</f>
-        <v>59127</v>
+        <v>77127</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added yacht to budget
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant\Desktop\Class Notes\Spring 2018\CS4320\CS4320TravelPlans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Documents/Software Engineering/CS4320TravelPlans/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,8 +14,11 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
   <si>
     <t>Travel</t>
   </si>
@@ -93,6 +96,9 @@
   </si>
   <si>
     <t>Vintage Philipponnat Clos</t>
+  </si>
+  <si>
+    <t>Yacht Rental</t>
   </si>
 </sst>
 </file>
@@ -455,11 +461,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
     <col min="2" max="3" width="22.6640625" customWidth="1"/>
@@ -543,12 +549,18 @@
       <c r="D4" s="3">
         <v>1855</v>
       </c>
+      <c r="E4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F4" s="4">
+        <v>8000</v>
+      </c>
       <c r="G4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="H4" s="2">
         <f>SUM(F4:F1048576)</f>
-        <v>0</v>
+        <v>8000</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
@@ -569,10 +581,10 @@
       </c>
       <c r="H5" s="2">
         <f>SUM($H2, $H3, $H4)</f>
-        <v>85864</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>93864</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C6" t="s">
         <v>15</v>
       </c>
@@ -580,7 +592,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>16</v>
       </c>
@@ -588,7 +600,7 @@
         <v>2400</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>17</v>
       </c>
@@ -596,7 +608,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>18</v>
       </c>
@@ -604,7 +616,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>19</v>
       </c>
@@ -612,7 +624,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>20</v>
       </c>
@@ -620,7 +632,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>21</v>
       </c>
@@ -628,7 +640,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Added penthouse to budget and itinerary
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
   <si>
     <t>Travel</t>
   </si>
@@ -99,6 +99,9 @@
   </si>
   <si>
     <t>Yacht Rental</t>
+  </si>
+  <si>
+    <t>Penthouse Rental</t>
   </si>
 </sst>
 </file>
@@ -462,7 +465,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -560,7 +563,7 @@
       </c>
       <c r="H4" s="2">
         <f>SUM(F4:F1048576)</f>
-        <v>8000</v>
+        <v>16323</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
@@ -576,12 +579,18 @@
       <c r="D5" s="4">
         <v>142</v>
       </c>
+      <c r="E5" t="s">
+        <v>24</v>
+      </c>
+      <c r="F5" s="3">
+        <v>8323</v>
+      </c>
       <c r="G5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="H5" s="2">
         <f>SUM($H2, $H3, $H4)</f>
-        <v>93864</v>
+        <v>102187</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Added helicopter ride to budget and itinerary
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>Travel</t>
   </si>
@@ -102,6 +102,9 @@
   </si>
   <si>
     <t>Penthouse Rental</t>
+  </si>
+  <si>
+    <t>Helicopter Ride</t>
   </si>
 </sst>
 </file>
@@ -465,7 +468,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -563,10 +566,10 @@
       </c>
       <c r="H4" s="2">
         <f>SUM(F4:F1048576)</f>
-        <v>16323</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+        <v>18128</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -590,7 +593,7 @@
       </c>
       <c r="H5" s="2">
         <f>SUM($H2, $H3, $H4)</f>
-        <v>102187</v>
+        <v>103992</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.2">
@@ -599,6 +602,12 @@
       </c>
       <c r="D6" s="4">
         <v>390</v>
+      </c>
+      <c r="E6" t="s">
+        <v>25</v>
+      </c>
+      <c r="F6" s="3">
+        <v>1805</v>
       </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
Updated budget and itinerary for the Justin Timberlake concert
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -1,11 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="27610"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/nathan/Documents/Software Engineering/CS4320TravelPlans/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant\Desktop\Class Notes\Spring 2018\CS4320\CS4320TravelPlans\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -14,11 +14,8 @@
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
-      <x14:workbookPr defaultImageDpi="32767"/>
-    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -27,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="27">
   <si>
     <t>Travel</t>
   </si>
@@ -105,6 +102,9 @@
   </si>
   <si>
     <t>Helicopter Ride</t>
+  </si>
+  <si>
+    <t>VIP Justin Timberlake Concert</t>
   </si>
 </sst>
 </file>
@@ -471,7 +471,7 @@
       <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
     <col min="2" max="3" width="22.6640625" customWidth="1"/>
@@ -566,10 +566,10 @@
       </c>
       <c r="H4" s="2">
         <f>SUM(F4:F1048576)</f>
-        <v>18128</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
+        <v>44373</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -593,10 +593,10 @@
       </c>
       <c r="H5" s="2">
         <f>SUM($H2, $H3, $H4)</f>
-        <v>103992</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+        <v>130237</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C6" t="s">
         <v>15</v>
       </c>
@@ -610,15 +610,21 @@
         <v>1805</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C7" t="s">
         <v>16</v>
       </c>
       <c r="D7" s="4">
         <v>2400</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="E7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F7" s="4">
+        <v>26245</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C8" t="s">
         <v>17</v>
       </c>
@@ -626,7 +632,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C9" t="s">
         <v>18</v>
       </c>
@@ -634,7 +640,7 @@
         <v>1025</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C10" t="s">
         <v>19</v>
       </c>
@@ -642,7 +648,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C11" t="s">
         <v>20</v>
       </c>
@@ -650,7 +656,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C12" t="s">
         <v>21</v>
       </c>
@@ -658,7 +664,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="C13" t="s">
         <v>22</v>
       </c>

</xml_diff>

<commit_message>
Updated the budget sheet for the stand up show
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
   <si>
     <t>Travel</t>
   </si>
@@ -111,6 +111,9 @@
   </si>
   <si>
     <t>Knick's Game</t>
+  </si>
+  <si>
+    <t>Stand Up Show</t>
   </si>
 </sst>
 </file>
@@ -474,7 +477,7 @@
   <dimension ref="A1:H13"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -572,7 +575,7 @@
       </c>
       <c r="H4" s="2">
         <f>SUM(F4:F1048576)</f>
-        <v>61961.75</v>
+        <v>62916.75</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
@@ -599,7 +602,7 @@
       </c>
       <c r="H5" s="2">
         <f>SUM($H2, $H3, $H4)</f>
-        <v>147825.75</v>
+        <v>148780.75</v>
       </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
@@ -664,6 +667,12 @@
       </c>
       <c r="D10" s="4">
         <v>750</v>
+      </c>
+      <c r="E10" t="s">
+        <v>29</v>
+      </c>
+      <c r="F10" s="3">
+        <v>955</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">

</xml_diff>

<commit_message>
Added mercedes rental plans
To get from Missouri to Chicago.
</commit_message>
<xml_diff>
--- a/Budget.xlsx
+++ b/Budget.xlsx
@@ -1,20 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10210"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\grant\Desktop\Class Notes\Spring 2018\CS4320\CS4320TravelPlans\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alex/Desktop/CS4320TravelPlans/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="7300" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="440" windowWidth="22160" windowHeight="11720" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511" concurrentCalc="0"/>
+  <calcPr calcId="171027" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="35" uniqueCount="31">
   <si>
     <t>Travel</t>
   </si>
@@ -114,12 +114,15 @@
   </si>
   <si>
     <t>Stand Up Show</t>
+  </si>
+  <si>
+    <t>Mercedes Rental</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
@@ -476,11 +479,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="24.83203125" customWidth="1"/>
     <col min="2" max="3" width="22.6640625" customWidth="1"/>
@@ -489,7 +492,7 @@
     <col min="7" max="7" width="18.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.7">
+    <row r="1" spans="1:8" ht="31" x14ac:dyDescent="0.35">
       <c r="A1" s="5" t="s">
         <v>3</v>
       </c>
@@ -503,7 +506,7 @@
       </c>
       <c r="H1" s="5"/>
     </row>
-    <row r="2" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
         <v>0</v>
       </c>
@@ -521,10 +524,10 @@
       </c>
       <c r="H2" s="2">
         <f>SUM(B4:B1048576)</f>
-        <v>77127</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+        <v>79627</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>9</v>
       </c>
@@ -551,7 +554,7 @@
         <v>8737</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>11</v>
       </c>
@@ -578,7 +581,7 @@
         <v>62916.75</v>
       </c>
     </row>
-    <row r="5" spans="1:8" ht="18.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:8" ht="19" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>12</v>
       </c>
@@ -602,10 +605,16 @@
       </c>
       <c r="H5" s="2">
         <f>SUM($H2, $H3, $H4)</f>
-        <v>148780.75</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+        <v>151280.75</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>30</v>
+      </c>
+      <c r="B6" s="4">
+        <v>2500</v>
+      </c>
       <c r="C6" t="s">
         <v>15</v>
       </c>
@@ -619,7 +628,7 @@
         <v>1805</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C7" t="s">
         <v>16</v>
       </c>
@@ -633,7 +642,7 @@
         <v>1762.5</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C8" t="s">
         <v>17</v>
       </c>
@@ -647,7 +656,7 @@
         <v>26245</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C9" t="s">
         <v>18</v>
       </c>
@@ -661,7 +670,7 @@
         <v>15826.25</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C10" t="s">
         <v>19</v>
       </c>
@@ -675,7 +684,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C11" t="s">
         <v>20</v>
       </c>
@@ -683,7 +692,7 @@
         <v>500</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C12" t="s">
         <v>21</v>
       </c>
@@ -691,7 +700,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="C13" t="s">
         <v>22</v>
       </c>

</xml_diff>